<commit_message>
fix all cases and changed case.excel
fix all cases and changed case.excel
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>TC_NO</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Secilen degerin sayfadan kayboldugu görülür.</t>
   </si>
   <si>
-    <t>Yapilacak_is_BirdenFazla_Ekleme</t>
-  </si>
-  <si>
     <t>* Eklenmis bir deger varken, Yeni bir deger girilir Enter'a basilir</t>
   </si>
   <si>
@@ -102,6 +99,30 @@
   </si>
   <si>
     <t>Secilen degerlerin sayfadan silindigi gorulur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yapilacak_is_Ekleme_All_Active_Completed </t>
+  </si>
+  <si>
+    <t>* What needs to be done ? İnput'u içerisine herhangi bir değer girilip Enter'a basılır bu islem 3 defa tekrarlanir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yazilan 3  değer başarılı şekilde eklendiği görülür,  X item left yazisi görülür , All Active Completed butonları görülür || Eklenen deger active olarak eklendigi gorulur </t>
+  </si>
+  <si>
+    <t>* 3 deger icerisinden 1. deger secilir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">* Active butonuna tiklanir </t>
+  </si>
+  <si>
+    <t>Secilmeyen degerlerin kaldigi görülur</t>
+  </si>
+  <si>
+    <t>* Completed butonuna tiklanir</t>
+  </si>
+  <si>
+    <t>Secilmeyen degerler ekrandan kaybolur , sadece secilen deger goruntulenir</t>
   </si>
 </sst>
 </file>
@@ -439,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -501,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -523,7 +544,7 @@
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -553,7 +574,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -561,7 +582,7 @@
         <v>14</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -583,7 +604,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -607,7 +628,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>5</v>
@@ -621,53 +642,69 @@
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
         <v>7</v>
       </c>
-      <c r="B18" t="s">
-        <v>23</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D19" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modified case 7 and changed all case names
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -38,36 +38,18 @@
     <t>TC_Excepted_Result</t>
   </si>
   <si>
-    <t>Todomvc_Sayfası</t>
-  </si>
-  <si>
     <t>* https://todomvc.com/examples/vue/#   adresine girilir</t>
   </si>
   <si>
     <t>Sayfanın Başarılı şekilde açıldıgı görülür</t>
   </si>
   <si>
-    <t>Yapilacak_is_Ekleme</t>
-  </si>
-  <si>
     <t>* What needs to be done ? İnput'u içerisine herhangi bir değer girilip Enter'a basılır</t>
   </si>
   <si>
     <t>* Seçilmeyen değerin yaninda bulunan X butonuna tıklanir.</t>
   </si>
   <si>
-    <t>Eğer birden fazla değer varsa, X items left yazisinin azaldigi görülür , Eğer bir tane deger varsa, All Acrive Completed butonlarinin kayboldugu görülür</t>
-  </si>
-  <si>
-    <t>Yapilacak_is_Ekleme_SecilerekSilme</t>
-  </si>
-  <si>
-    <t>Yapilacak_is_Ekleme_SecilmedenSilme</t>
-  </si>
-  <si>
-    <t>Yapilacak_is_Ekleme_Secme</t>
-  </si>
-  <si>
     <t>* Yazilen deger'in yanında bulunan radio button'a tiklanir</t>
   </si>
   <si>
@@ -92,18 +74,12 @@
     <t>X items left degerinin azaldigi görülür , yazinin secildigi görülür. Clear Completed butonu aktiflesir</t>
   </si>
   <si>
-    <t>Yapilacak_is_BirdenFazla_Ekleme_ClearCompleted</t>
-  </si>
-  <si>
     <t>* Birinci ve ikinci degerler secilir, Clear Compeleted butonuna tiklanir</t>
   </si>
   <si>
     <t>Secilen degerlerin sayfadan silindigi gorulur</t>
   </si>
   <si>
-    <t xml:space="preserve">Yapilacak_is_Ekleme_All_Active_Completed </t>
-  </si>
-  <si>
     <t>* What needs to be done ? İnput'u içerisine herhangi bir değer girilip Enter'a basılır bu islem 3 defa tekrarlanir</t>
   </si>
   <si>
@@ -123,6 +99,30 @@
   </si>
   <si>
     <t>Secilmeyen degerler ekrandan kaybolur , sadece secilen deger goruntulenir</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issue</t>
+  </si>
+  <si>
+    <t>Todomvc_Page_Display</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issue_Unselect_Remove</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issue_Select</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issue_select_Remove</t>
+  </si>
+  <si>
+    <t>Todo_Add_MoreIssues_ClearCompleted button</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issue_All-Active-Completed buttons</t>
+  </si>
+  <si>
+    <t>Eğer birden fazla değer varsa, X items left yazisinin azaldigi görülür , Eğer bir tane deger varsa, All Active Completed butonlarinin kayboldugu görülür</t>
   </si>
 </sst>
 </file>
@@ -462,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,13 +494,13 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -508,21 +508,21 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -530,29 +530,29 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="C5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C7" s="4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -560,29 +560,29 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C9" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C10" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -590,37 +590,37 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C12" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C13" s="4" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C14" s="4" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -628,37 +628,37 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C15" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C16" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C17" s="4" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C18" s="4" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,45 +666,45 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>5</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="C20" s="4" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C21" s="4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C22" s="4" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added 8. scenario and maintenance
</commit_message>
<xml_diff>
--- a/TestCases.xlsx
+++ b/TestCases.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>TC_NO</t>
   </si>
@@ -123,6 +123,21 @@
   </si>
   <si>
     <t>Eğer birden fazla değer varsa, X items left yazisinin azaldigi görülür , Eğer bir tane deger varsa, All Active Completed butonlarinin kayboldugu görülür</t>
+  </si>
+  <si>
+    <t>Todo_Add_Issueses_Random_SelectDone</t>
+  </si>
+  <si>
+    <t>* What needs to be done ? İnput'u içerisine herhangi bir değer girilip Enter'a basılır bu islem birden fazla olucak sekilde defa tekrarlanir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yazilan  değerler başarılı şekilde eklendiği görülür,  X item left yazisi görülür , All Active Completed butonları görülür || Eklenen deger active olarak eklendigi gorulur </t>
+  </si>
+  <si>
+    <t>* Rastgele 1 issue'nun yanındaki checkBox tiklanir</t>
+  </si>
+  <si>
+    <t>Tıklanilan issue DONE statüsüne geldigi gorulur</t>
   </si>
 </sst>
 </file>
@@ -460,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,6 +722,36 @@
         <v>24</v>
       </c>
     </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="C25" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>